<commit_message>
fixing spark lab scripts / instructions
</commit_message>
<xml_diff>
--- a/5-sql/Benchmarking_Dataformats.xlsx
+++ b/5-sql/Benchmarking_Dataformats.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22300" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="sample results" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="11">
   <si>
     <t>parquet</t>
   </si>
@@ -290,7 +291,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>39.4311</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -308,11 +309,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2118287976"/>
-        <c:axId val="2140532520"/>
+        <c:axId val="2130023288"/>
+        <c:axId val="2130026232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2118287976"/>
+        <c:axId val="2130023288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -321,7 +322,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2140532520"/>
+        <c:crossAx val="2130026232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -329,7 +330,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140532520"/>
+        <c:axId val="2130026232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -340,7 +341,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118287976"/>
+        <c:crossAx val="2130023288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -406,10 +407,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>25.78</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.592</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -424,11 +425,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2143572472"/>
-        <c:axId val="-2115526280"/>
+        <c:axId val="2130103304"/>
+        <c:axId val="2130106248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2143572472"/>
+        <c:axId val="2130103304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -437,7 +438,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115526280"/>
+        <c:crossAx val="2130106248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -445,7 +446,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115526280"/>
+        <c:axId val="2130106248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -456,7 +457,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143572472"/>
+        <c:crossAx val="2130103304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -533,13 +534,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1415.188092</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80.667991</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -554,11 +555,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2119405624"/>
-        <c:axId val="-2141871336"/>
+        <c:axId val="2129833144"/>
+        <c:axId val="2129836088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2119405624"/>
+        <c:axId val="2129833144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -567,7 +568,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2141871336"/>
+        <c:crossAx val="2129836088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -575,7 +576,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2141871336"/>
+        <c:axId val="2129836088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -586,7 +587,390 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119405624"/>
+        <c:crossAx val="2129833144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.148012745905603"/>
+          <c:y val="0.0552147505988844"/>
+          <c:w val="0.851987254094397"/>
+          <c:h val="0.647116877018925"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'sample results'!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>time (secs)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'sample results'!$A$5:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>json</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>compressed json</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>parquet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'sample results'!$B$5:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>39.4311</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2129849928"/>
+        <c:axId val="2130165096"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2129849928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2130165096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2130165096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2129849928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'sample results'!$A$12:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>json</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>compressed json</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>parquet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'sample results'!$B$12:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>25.78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.592</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2130720280"/>
+        <c:axId val="2130723224"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2130720280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2130723224"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2130723224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2130720280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'sample results'!$C$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>size (MB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'sample results'!$A$20:$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>json</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>compressed json</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>parquet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'sample results'!$C$20:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1415.188092</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80.667991</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2131295736"/>
+        <c:axId val="2086800584"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2131295736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2086800584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2086800584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2131295736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -682,6 +1066,107 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>770470</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>220135</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>67733</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>25399</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>262466</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>338666</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>16933</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>110066</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1022,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1050,6 +1535,167 @@
         <v>4</v>
       </c>
       <c r="B5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="25">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="25">
+      <c r="A18" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <f>B20/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f>B20/1000000000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21">
+        <f t="shared" ref="C21:C22" si="0">B21/1000000</f>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:D22" si="1">B21/1000000000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:D22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" ht="23">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
         <v>39.431100000000001</v>
       </c>
     </row>

</xml_diff>